<commit_message>
20211118 se agrega base de datos con modificacion a tabla asignatura, se agrga columna color, se agrega api con modelo que administra columna color, se modifica en el esquema, se edita excel api con parametros optativa_container y optativa_categorias
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djanr2\Desktop\DOCUMENTACION UNAM FI ASIGNATURAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37436B3A-CC81-4728-A113-7D36989BFFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B64D5-0561-4C7E-9A85-CEC40A127564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1095" windowWidth="29040" windowHeight="15465" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENDPOINTS" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="173">
   <si>
     <t>OPERACION</t>
   </si>
@@ -575,7 +575,37 @@
     <t>getInfoMapaCurricular</t>
   </si>
   <si>
-    <t>PENDIENTE</t>
+    <t>optativa_container</t>
+  </si>
+  <si>
+    <t>optativa_categorias</t>
+  </si>
+  <si>
+    <r>
+      <t>Obtendrá la información necesaria para elaborar el mapa curricular en formato .json, con base a los parametros de {year} y {carrera}. 
+Se considera como la</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> version 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>del Api ya que se agreega ingormacion como las barras, notas, suma_creditos_pensum_academico optativa_container y optativa_categoria</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -954,39 +984,39 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1140,6 +1170,12 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1149,12 +1185,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1182,7 +1212,9 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Énfasis1" xfId="3" builtinId="30"/>
@@ -1474,8 +1506,8 @@
   </sheetPr>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2328,7 @@
     </row>
     <row r="36" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
-        <v>170</v>
+        <v>102</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>167</v>
@@ -2318,7 +2350,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
+      <c r="A37" s="31"/>
       <c r="E37"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2435,10 +2467,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="58" t="s">
@@ -2452,8 +2484,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="98"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="100"/>
       <c r="C3" s="59"/>
       <c r="D3" s="1" t="s">
         <v>22</v>
@@ -2463,8 +2495,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="98"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="59"/>
       <c r="D4" s="1" t="s">
         <v>24</v>
@@ -2474,8 +2506,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="98"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="59"/>
       <c r="D5" s="1" t="s">
         <v>23</v>
@@ -2485,7 +2517,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="97"/>
       <c r="C6" s="59"/>
       <c r="D6" s="1" t="s">
@@ -2496,10 +2528,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="39" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="59"/>
@@ -2509,8 +2541,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="59"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -2518,8 +2550,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="98"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="59"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -2527,8 +2559,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="98"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="100"/>
       <c r="C10" s="59"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -2536,7 +2568,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="97"/>
       <c r="C11" s="59"/>
       <c r="D11" s="1"/>
@@ -2545,10 +2577,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="39" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="59"/>
@@ -2558,8 +2590,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="98"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="59"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
@@ -2567,8 +2599,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="98"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="59"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
@@ -2576,8 +2608,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="98"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="100"/>
       <c r="C15" s="59"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -2585,7 +2617,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="97"/>
       <c r="C16" s="60"/>
       <c r="D16" s="1"/>
@@ -2724,7 +2756,7 @@
       <c r="A30" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="101" t="s">
+      <c r="B30" s="98" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="90" t="s">
@@ -2739,7 +2771,7 @@
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="95"/>
-      <c r="B31" s="102"/>
+      <c r="B31" s="99"/>
       <c r="C31" s="91"/>
       <c r="D31" s="3" t="s">
         <v>22</v>
@@ -2750,7 +2782,7 @@
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="95"/>
-      <c r="B32" s="102"/>
+      <c r="B32" s="99"/>
       <c r="C32" s="91"/>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2759,7 +2791,7 @@
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="95"/>
-      <c r="B33" s="102"/>
+      <c r="B33" s="99"/>
       <c r="C33" s="91"/>
       <c r="D33" s="3" t="s">
         <v>21</v>
@@ -2768,7 +2800,7 @@
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="95"/>
-      <c r="B34" s="102"/>
+      <c r="B34" s="99"/>
       <c r="C34" s="91"/>
       <c r="D34" s="3" t="s">
         <v>27</v>
@@ -2777,7 +2809,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="95"/>
-      <c r="B35" s="102"/>
+      <c r="B35" s="99"/>
       <c r="C35" s="91"/>
       <c r="D35" s="3" t="s">
         <v>28</v>
@@ -2786,7 +2818,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="95"/>
-      <c r="B36" s="102"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="91"/>
       <c r="D36" s="3" t="s">
         <v>29</v>
@@ -2795,7 +2827,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="95"/>
-      <c r="B37" s="102"/>
+      <c r="B37" s="99"/>
       <c r="C37" s="91"/>
       <c r="D37" s="3" t="s">
         <v>30</v>
@@ -2804,7 +2836,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="95"/>
-      <c r="B38" s="102"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="91"/>
       <c r="D38" s="3" t="s">
         <v>31</v>
@@ -2813,7 +2845,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="95"/>
-      <c r="B39" s="102"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="91"/>
       <c r="D39" s="3" t="s">
         <v>32</v>
@@ -2822,7 +2854,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="95"/>
-      <c r="B40" s="102"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="91"/>
       <c r="D40" s="3" t="s">
         <v>20</v>
@@ -2831,7 +2863,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="95"/>
-      <c r="B41" s="102"/>
+      <c r="B41" s="99"/>
       <c r="C41" s="91"/>
       <c r="D41" s="3" t="s">
         <v>33</v>
@@ -2944,10 +2976,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>154</v>
       </c>
       <c r="C2" s="105" t="s">
@@ -2962,8 +2994,8 @@
       <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="105"/>
       <c r="D3" s="1" t="s">
         <v>24</v>
@@ -2973,8 +3005,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="105"/>
       <c r="D4" s="33"/>
       <c r="E4" s="1" t="s">
@@ -2982,8 +3014,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="105"/>
       <c r="D5" s="33"/>
       <c r="E5" s="1" t="s">
@@ -2991,8 +3023,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="105"/>
       <c r="D6" s="33"/>
       <c r="E6" s="1" t="s">
@@ -3028,10 +3060,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,12 +3094,12 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="106" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B2" s="109" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="32" t="s">
@@ -3080,7 +3112,7 @@
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="107"/>
       <c r="B3" s="110"/>
-      <c r="C3" s="39"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="32" t="s">
         <v>24</v>
       </c>
@@ -3091,71 +3123,83 @@
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="107"/>
       <c r="B4" s="110"/>
-      <c r="C4" s="39"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="33"/>
       <c r="E4" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="107"/>
       <c r="B5" s="110"/>
-      <c r="C5" s="39"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="33"/>
       <c r="E5" s="32" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="107"/>
       <c r="B6" s="110"/>
-      <c r="C6" s="39"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="33"/>
       <c r="E6" s="32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="107"/>
       <c r="B7" s="110"/>
-      <c r="C7" s="39"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="34"/>
       <c r="E7" s="32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="107"/>
       <c r="B8" s="110"/>
-      <c r="C8" s="39"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="34"/>
       <c r="E8" s="32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="107"/>
       <c r="B9" s="110"/>
-      <c r="C9" s="39"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="34"/>
-      <c r="E9" s="32" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="108"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="40"/>
+      <c r="E9" s="112" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="34"/>
       <c r="E10" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="108"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="32" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C2:C11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{5D639DF4-4055-4D54-B35A-0CEFA31F77BE}"/>
@@ -3203,13 +3247,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3220,36 +3264,36 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="39"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="40"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -3307,13 +3351,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3324,9 +3368,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3335,31 +3379,31 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="40"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -3422,7 +3466,7 @@
       <c r="A2" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="58" t="s">
@@ -3486,7 +3530,7 @@
       <c r="A8" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="59"/>
@@ -3925,13 +3969,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3942,40 +3986,40 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="40"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -4158,13 +4202,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4175,9 +4219,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="97"/>
-      <c r="C3" s="39"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
@@ -4186,13 +4230,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
@@ -4201,9 +4245,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="97"/>
-      <c r="C5" s="39"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
@@ -4212,22 +4256,22 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="39"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="97"/>
-      <c r="C7" s="40"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>11</v>
@@ -4431,13 +4475,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4448,9 +4492,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="97"/>
-      <c r="C3" s="39"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
@@ -4459,13 +4503,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
@@ -4474,40 +4518,40 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
+      <c r="A5" s="102"/>
       <c r="B5" s="97"/>
-      <c r="C5" s="39"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="39"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="97"/>
-      <c r="C8" s="40"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>153</v>
@@ -4563,7 +4607,7 @@
       <c r="A13" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="98" t="s">
         <v>84</v>
       </c>
       <c r="C13" s="90" t="s">
@@ -4578,7 +4622,7 @@
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="95"/>
-      <c r="B14" s="102"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="91"/>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -4589,7 +4633,7 @@
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="95"/>
-      <c r="B15" s="102"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="91"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -4598,7 +4642,7 @@
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="95"/>
-      <c r="B16" s="102"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="91"/>
       <c r="D16" s="3" t="s">
         <v>21</v>
@@ -4607,7 +4651,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="95"/>
-      <c r="B17" s="102"/>
+      <c r="B17" s="99"/>
       <c r="C17" s="91"/>
       <c r="D17" s="3" t="s">
         <v>23</v>
@@ -4644,6 +4688,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C13:C17"/>
@@ -4653,13 +4704,6 @@
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{19766D17-2256-47E9-986D-0001E3F5E42D}"/>

</xml_diff>

<commit_message>
20220221 se agregan documentacion de nuevas tablas, actualizacion de datos, actualizacion de api
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djanr2\Desktop\DOCUMENTACION UNAM FI ASIGNATURAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B64D5-0561-4C7E-9A85-CEC40A127564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF09CF-C5DB-44B4-9584-B5F7289F2181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1095" windowWidth="29040" windowHeight="15465" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENDPOINTS" sheetId="9" r:id="rId1"/>
@@ -23,8 +23,13 @@
     <sheet name="SERIACION" sheetId="7" r:id="rId8"/>
     <sheet name="CARRERA" sheetId="6" r:id="rId9"/>
     <sheet name="ASIGNATURA" sheetId="8" r:id="rId10"/>
-    <sheet name="MAPA_CURRICULAR" sheetId="12" r:id="rId11"/>
-    <sheet name="INFORMACION MAPA" sheetId="13" r:id="rId12"/>
+    <sheet name="NOTA_MAPA" sheetId="14" r:id="rId11"/>
+    <sheet name="OPTATIVA_ASIGNATURA" sheetId="15" r:id="rId12"/>
+    <sheet name="OPTATIVA_CATEGORIA" sheetId="16" r:id="rId13"/>
+    <sheet name="OPTATIVA_CONTAINER" sheetId="17" r:id="rId14"/>
+    <sheet name="OPTATIVA_TABLA" sheetId="18" r:id="rId15"/>
+    <sheet name="MAPA_CURRICULAR" sheetId="12" r:id="rId16"/>
+    <sheet name="INFORMACION MAPA" sheetId="13" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ENDPOINTS!$A$1:$G$34</definedName>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="249">
   <si>
     <t>OPERACION</t>
   </si>
@@ -606,6 +611,234 @@
       </rPr>
       <t>del Api ya que se agreega ingormacion como las barras, notas, suma_creditos_pensum_academico optativa_container y optativa_categoria</t>
     </r>
+  </si>
+  <si>
+    <t>NotasMapaController</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}</t>
+  </si>
+  <si>
+    <t>postNotas</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/nota</t>
+  </si>
+  <si>
+    <t>Insertará un registro de tipo NotaMapa, a tabla Nota_mapa</t>
+  </si>
+  <si>
+    <t>Actualizará la información del registro especificado mediante el parámetro {id} registro de la tabla Nota_mapa</t>
+  </si>
+  <si>
+    <t>Eliminará el registro especificado mediante el parámetro {id} de la tabla Nota_mapa</t>
+  </si>
+  <si>
+    <t>patchNota</t>
+  </si>
+  <si>
+    <t>deleteNota</t>
+  </si>
+  <si>
+    <t>getNotasById</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/nota/{id}</t>
+  </si>
+  <si>
+    <t>Obtendrá el registro especificado mediante el parámetro {id} de la tabla Nota_mapa, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>Obtendrá los registros de la tabla Nota_mapa con base en los parámetros {year} y {carrera}, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/nota/{year}/{carrera}</t>
+  </si>
+  <si>
+    <t>getNotaByYearAndCarrera</t>
+  </si>
+  <si>
+    <t>simbolo</t>
+  </si>
+  <si>
+    <t>leyenda</t>
+  </si>
+  <si>
+    <t>OptativaAsignaturaController</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/asignatura/{id}</t>
+  </si>
+  <si>
+    <t>getOptativaAsignaturaById</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/container/categoria/tabla/{id}/asignatura</t>
+  </si>
+  <si>
+    <t>getOptativaAsignaturaTabla</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/asignatura/{id}</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/asignatura</t>
+  </si>
+  <si>
+    <t>Insertará un registro de tipo OptaivaAsignatura, a tabla Optativa_asignatura</t>
+  </si>
+  <si>
+    <t>Actualizará la información del registro especificado mediante el parámetro {id} registro de la tabla Optativa_asignatura</t>
+  </si>
+  <si>
+    <t>Eliminará el registro especificado mediante el parámetro {id} de la tabla Optativa_asignatura</t>
+  </si>
+  <si>
+    <t>Obtendrá el registro especificado mediante el parámetro {id} de la tabla Optativa_asignatura, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>tabla</t>
+  </si>
+  <si>
+    <t>OptativaCategoriaController</t>
+  </si>
+  <si>
+    <t>deleteCategoria</t>
+  </si>
+  <si>
+    <t>patchCategoria</t>
+  </si>
+  <si>
+    <t>postCategoria</t>
+  </si>
+  <si>
+    <t>getOptativaCategoriaContainer</t>
+  </si>
+  <si>
+    <t>getOptativaCategoria</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/categoria/{id}</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/categoria</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/container/{id}/categoria</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/categoria/{id}</t>
+  </si>
+  <si>
+    <t>Insertará un registro de tipo OptaivaCategoria, a tabla Optativa_Categoria</t>
+  </si>
+  <si>
+    <t>Actualizará la información del registro especificado mediante el parámetro {id} registro de la tabla Optativa_Categoria</t>
+  </si>
+  <si>
+    <t>Eliminará el registro especificado mediante el parámetro {id} de la tabla Optativa_Categoria</t>
+  </si>
+  <si>
+    <t>Obtendrá el registro especificado mediante el parámetro {id} de la tabla Optativa_Categoria, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>nota_mapa</t>
+  </si>
+  <si>
+    <t>optativa_asignatura</t>
+  </si>
+  <si>
+    <t>optativa_categoria</t>
+  </si>
+  <si>
+    <t>OptativaContainerController</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/container/{id}</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/container/{year}/{carrera}</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/container/{id}</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/container</t>
+  </si>
+  <si>
+    <t>Insertará un registro de tipo OptaivaCategoria, a tabla Optativa_Container</t>
+  </si>
+  <si>
+    <t>Actualizará la información del registro especificado mediante el parámetro {id} registro de la tabla Optativa_Container</t>
+  </si>
+  <si>
+    <t>Eliminará el registro especificado mediante el parámetro {id} de la tabla Optativa_Container</t>
+  </si>
+  <si>
+    <t>Obtendrá el registro especificado mediante el parámetro {id} de la tabla Optativa_Container, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>Obtendrá los registros de la tabla Optativa_Container con base en los parámetros {year} y {carrera}, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>deleteContainer</t>
+  </si>
+  <si>
+    <t>patchContainer</t>
+  </si>
+  <si>
+    <t>postContainer</t>
+  </si>
+  <si>
+    <t>getOptativaContainerByCarrera</t>
+  </si>
+  <si>
+    <t>getOptativaContainerById</t>
+  </si>
+  <si>
+    <t>OptativaTablaController</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/tabla/{id}</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/api/optativa/container/categoria/{id}/tabla</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/tabla</t>
+  </si>
+  <si>
+    <t>https://asignaturas.fi.unam.api:8080/admin/api/optativa/tabla/{id}</t>
+  </si>
+  <si>
+    <t>Insertará un registro de tipo OptaivaCategoria, a tabla Optativa_tabla</t>
+  </si>
+  <si>
+    <t>Actualizará la información del registro especificado mediante el parámetro {id} registro de la tabla Optativa_tabla</t>
+  </si>
+  <si>
+    <t>Eliminará el registro especificado mediante el parámetro {id} de la tabla Optativa_tabla</t>
+  </si>
+  <si>
+    <t>Obtendrá el registro especificado mediante el parámetro {id} de la tabla Optativa_tabla, obtenidos en formato .json</t>
+  </si>
+  <si>
+    <t>getOptativaTablaById</t>
+  </si>
+  <si>
+    <t>getOptativaTablaCategoria</t>
+  </si>
+  <si>
+    <t>postTabla</t>
+  </si>
+  <si>
+    <t>patchTabla</t>
+  </si>
+  <si>
+    <t>deleteTabla</t>
+  </si>
+  <si>
+    <t>optativa_tabla</t>
   </si>
 </sst>
 </file>
@@ -879,7 +1112,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -984,6 +1217,12 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1170,21 +1409,21 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1212,8 +1451,83 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1504,17 +1818,17 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="28"/>
     <col min="6" max="6" width="28.140625" customWidth="1"/>
@@ -1557,21 +1871,21 @@
       <c r="D2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="36" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="34" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -1580,7 +1894,7 @@
       <c r="D3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -1591,10 +1905,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="34" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -1603,13 +1917,13 @@
       <c r="D4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="36" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1626,13 +1940,13 @@
       <c r="D5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="36" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1649,7 +1963,7 @@
       <c r="D6" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F6" s="11" t="s">
@@ -1787,7 +2101,7 @@
       <c r="D12" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F12" s="11" t="s">
@@ -1798,10 +2112,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -1810,7 +2124,7 @@
       <c r="D13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F13" s="11" t="s">
@@ -1890,10 +2204,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="34" t="s">
         <v>73</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -1902,21 +2216,21 @@
       <c r="D17" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="36" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="34" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -1925,7 +2239,7 @@
       <c r="D18" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F18" s="11" t="s">
@@ -1936,10 +2250,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="34" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -1948,7 +2262,7 @@
       <c r="D19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="11" t="s">
@@ -2040,7 +2354,7 @@
       <c r="D23" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F23" s="11" t="s">
@@ -2063,7 +2377,7 @@
       <c r="D24" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="36" t="s">
         <v>92</v>
       </c>
       <c r="F24" s="11" t="s">
@@ -2086,13 +2400,13 @@
       <c r="D25" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="36" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2166,10 +2480,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="34" t="s">
         <v>80</v>
       </c>
       <c r="C29" s="17" t="s">
@@ -2178,21 +2492,21 @@
       <c r="D29" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="36" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="34" t="s">
         <v>79</v>
       </c>
       <c r="C30" s="17" t="s">
@@ -2201,13 +2515,13 @@
       <c r="D30" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="36" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2224,13 +2538,13 @@
       <c r="D31" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="36" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2316,7 +2630,7 @@
       <c r="D35" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="32" t="s">
         <v>92</v>
       </c>
       <c r="F35" s="35" t="s">
@@ -2339,7 +2653,7 @@
       <c r="D36" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="32" t="s">
         <v>92</v>
       </c>
       <c r="F36" s="35" t="s">
@@ -2349,42 +2663,580 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="E37"/>
-    </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E39"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E40"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E41"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E42"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E43"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E44"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E45"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E46"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E47"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E48"/>
+    <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="G45" s="35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="G46" s="35" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A50" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="G50" s="35" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" s="35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A55" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="G55" s="35" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A56" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="G56" s="35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A60" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="G60" s="35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A61" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="G61" s="35" t="s">
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G34" xr:uid="{044CBF4E-5BB3-42D9-ABAA-C137E3B7EBB0}"/>
@@ -2423,9 +3275,34 @@
     <hyperlink ref="C25" r:id="rId32" xr:uid="{05B9EA1B-CB50-4BD3-A905-3A082245342B}"/>
     <hyperlink ref="C31" r:id="rId33" xr:uid="{A850496D-0F43-4FF2-9824-32790A835414}"/>
     <hyperlink ref="C35" r:id="rId34" xr:uid="{8092D904-E8C1-4765-A554-6FEBC1418319}"/>
+    <hyperlink ref="C37" r:id="rId35" xr:uid="{C928FF85-2BE2-4FFC-8BC8-D169C9821364}"/>
+    <hyperlink ref="C38" r:id="rId36" xr:uid="{CCE17A37-FD8D-4849-8634-D708872C9509}"/>
+    <hyperlink ref="C39" r:id="rId37" xr:uid="{EF1EC69A-BCC1-4D00-AA71-BEDCFAF23E97}"/>
+    <hyperlink ref="C40" r:id="rId38" xr:uid="{9BB70596-2281-417A-B981-EBC27E94CAC4}"/>
+    <hyperlink ref="C41" r:id="rId39" xr:uid="{7302396E-3098-4751-A46B-7D2C067F4E10}"/>
+    <hyperlink ref="C42" r:id="rId40" xr:uid="{1070821A-D0A0-4F9F-BB4D-E049CFEA86D4}"/>
+    <hyperlink ref="C43" r:id="rId41" xr:uid="{9007FA0A-B0DA-45C7-8F4A-C426DAFEC26B}"/>
+    <hyperlink ref="C44" r:id="rId42" xr:uid="{B8FE5338-48A9-4F61-A96A-A7438B13241E}"/>
+    <hyperlink ref="C45" r:id="rId43" xr:uid="{12414C90-A1C9-4596-84F9-0F191BA05FFF}"/>
+    <hyperlink ref="C46" r:id="rId44" xr:uid="{B41BDBE9-375B-4385-9D8A-4BDBE0215D45}"/>
+    <hyperlink ref="C47" r:id="rId45" xr:uid="{3630E8E5-DDBC-4A91-A698-DCA4C582E7DC}"/>
+    <hyperlink ref="C48" r:id="rId46" xr:uid="{1C011E94-912D-47B5-9CEC-36E438F6920F}"/>
+    <hyperlink ref="C49" r:id="rId47" xr:uid="{5135296A-A534-42A0-BF0A-0CDA54BD8E6D}"/>
+    <hyperlink ref="C50" r:id="rId48" xr:uid="{7E1D6D76-F668-48E9-A38D-D7DF57EC5ED0}"/>
+    <hyperlink ref="C51" r:id="rId49" xr:uid="{E394D885-06DB-43D3-8F16-7D87A1CBF178}"/>
+    <hyperlink ref="C52" r:id="rId50" xr:uid="{0C1D4EB5-CAF7-4CE3-B9CA-E0888F136F2D}"/>
+    <hyperlink ref="C54" r:id="rId51" xr:uid="{419100E0-561A-4F21-8B69-35D42E4A7991}"/>
+    <hyperlink ref="C55" r:id="rId52" xr:uid="{019EFC4B-C748-484C-B0EB-A2123F38C4D7}"/>
+    <hyperlink ref="C56" r:id="rId53" xr:uid="{15853290-B7D7-4E43-9B0B-7877BD6A59F6}"/>
+    <hyperlink ref="C53" r:id="rId54" xr:uid="{44BB601F-D285-4FA1-9D5E-9BABFD893B1D}"/>
+    <hyperlink ref="C57" r:id="rId55" xr:uid="{C7EA180C-1B0D-4FB7-BF44-F615FFE70CD8}"/>
+    <hyperlink ref="C58" r:id="rId56" xr:uid="{3F3CAF9E-53F3-424B-8B47-82DD7AAC4E27}"/>
+    <hyperlink ref="C59" r:id="rId57" xr:uid="{EDEC7BA5-2CEB-43D4-8F6B-03CC1BDBACFB}"/>
+    <hyperlink ref="C60" r:id="rId58" xr:uid="{0F087AB8-27F2-433C-8865-66D518149B4D}"/>
+    <hyperlink ref="C61" r:id="rId59" xr:uid="{98D62C46-57CF-47B8-BA04-1E9EBDF6639A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 
@@ -2467,13 +3344,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="60" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2484,9 +3361,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="100"/>
-      <c r="C3" s="59"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2495,9 +3372,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="100"/>
-      <c r="C4" s="59"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2506,9 +3383,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="100"/>
-      <c r="C5" s="59"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
@@ -2517,9 +3394,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="97"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2528,111 +3405,111 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="59"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="100"/>
-      <c r="C8" s="59"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="100"/>
-      <c r="C9" s="59"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="100"/>
-      <c r="C10" s="59"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="97"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="59"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="100"/>
-      <c r="C13" s="59"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="100"/>
-      <c r="C14" s="59"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="100"/>
-      <c r="C15" s="59"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="97"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -2643,9 +3520,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="81"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="69"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="71"/>
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2654,112 +3531,112 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="81"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="69"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="69"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="81"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="69"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="81"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="69"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="71"/>
       <c r="D22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="81"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="69"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="69"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="69"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="69"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="69"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="69"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="70"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="94" t="s">
+      <c r="A30" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="90" t="s">
+      <c r="C30" s="92" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2770,9 +3647,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="95"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="91"/>
+      <c r="A31" s="97"/>
+      <c r="B31" s="104"/>
+      <c r="C31" s="93"/>
       <c r="D31" s="3" t="s">
         <v>22</v>
       </c>
@@ -2781,112 +3658,112 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="91"/>
+      <c r="A32" s="97"/>
+      <c r="B32" s="104"/>
+      <c r="C32" s="93"/>
       <c r="D32" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="91"/>
+      <c r="A33" s="97"/>
+      <c r="B33" s="104"/>
+      <c r="C33" s="93"/>
       <c r="D33" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="91"/>
+      <c r="A34" s="97"/>
+      <c r="B34" s="104"/>
+      <c r="C34" s="93"/>
       <c r="D34" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="95"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="91"/>
+      <c r="A35" s="97"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="93"/>
       <c r="D35" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="95"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="91"/>
+      <c r="A36" s="97"/>
+      <c r="B36" s="104"/>
+      <c r="C36" s="93"/>
       <c r="D36" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="95"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="91"/>
+      <c r="A37" s="97"/>
+      <c r="B37" s="104"/>
+      <c r="C37" s="93"/>
       <c r="D37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="95"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="91"/>
+      <c r="A38" s="97"/>
+      <c r="B38" s="104"/>
+      <c r="C38" s="93"/>
       <c r="D38" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="95"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="91"/>
+      <c r="A39" s="97"/>
+      <c r="B39" s="104"/>
+      <c r="C39" s="93"/>
       <c r="D39" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="95"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="91"/>
+      <c r="A40" s="97"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="93"/>
       <c r="D40" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="95"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="91"/>
+      <c r="A41" s="97"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="93"/>
       <c r="D41" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="96"/>
-      <c r="B42" s="104"/>
-      <c r="C42" s="103"/>
+      <c r="A42" s="98"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="105"/>
       <c r="D42" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="77" t="s">
+      <c r="A43" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="75" t="s">
+      <c r="C43" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -2897,9 +3774,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="78"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="76"/>
+      <c r="A44" s="80"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="78"/>
       <c r="D44" s="4" t="s">
         <v>8</v>
       </c>
@@ -2939,6 +3816,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1518901-C313-4E7C-9189-94974702DDCE}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="A2:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="115" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="125" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="116"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="117"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="115" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="116"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="116"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="117"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="118" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="128" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="119"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="119"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="119"/>
+      <c r="B12" s="129"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="120" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="130" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="121"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="122"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="123" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="133" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="124"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="114"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="A5:A8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{6F51F9CF-1100-47E2-B533-1C509854EFEA}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{0A81ED79-ABF8-49B9-AC0D-0BE64057895C}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{4B4FDF34-67CA-49B8-8E91-FB457B0AD6D7}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{4469C42C-32E6-43D4-A36D-8DF15805A53E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7138B7-8853-42DB-B813-B009524BB1F0}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="135"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="118" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="128" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="119"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="137"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="120" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="130" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="121"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="122"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="123" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="124"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="https://asignaturas.fi.unam.api:8080/admin/api/nota" xr:uid="{5DA58BD4-852E-4577-974B-9EC7C86771A9}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{4BFEC48C-DD78-4EF4-BF48-96937CF4D3AA}"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{7C847B32-3A62-408A-9F30-4C3A615BFF1F}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://asignaturas.fi.unam.api:8080/api/nota/{id}" xr:uid="{65E744D3-F60C-4CA3-8E4A-71C0AE19D03B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF22E21-5DEA-473D-8F5A-5CE87E2C70DE}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="135"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="135" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="118" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="128" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="119"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="137"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="120" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="121"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="122"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="123" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="124"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="https://asignaturas.fi.unam.api:8080/admin/api/nota" xr:uid="{9939DBBB-96C8-429E-9893-8BFBA513796C}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{71A1B687-1F98-48BE-A56B-8852AB3BC975}"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{6EA2C46C-B331-47CF-81DB-07D7C9052B72}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://asignaturas.fi.unam.api:8080/api/nota/{id}" xr:uid="{D6E46C43-E84E-4824-AE1A-21714138CA34}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0462B0D-474B-4B24-A939-80EE88A954FE}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="97.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="135"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="135" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="118" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="128" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="119"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="137"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="120" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="130" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="121"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="122"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="123" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="124"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="https://asignaturas.fi.unam.api:8080/admin/api/nota" xr:uid="{B79F204D-3A5A-4888-AE2E-9C9CB4D32E27}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{59D730F2-1FDB-4DF1-9451-A6245B5C9C6D}"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{DBB8343E-5041-456C-99D0-2DDCDD54BF7C}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://asignaturas.fi.unam.api:8080/api/nota/{id}" xr:uid="{98828699-D7CB-4CA7-8D30-D599D61B86E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927B7E7-41DE-49CA-B823-259BD82C8545}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
+    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="135" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="135"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="135" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="118" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="128" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="119"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="137"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="120" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" s="130" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="121"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="122"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="123" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="124"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="https://asignaturas.fi.unam.api:8080/admin/api/nota" xr:uid="{FD029BBF-6D38-4604-9EC1-57328C6293B5}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{D78103A8-C004-4E99-9EA9-EBFFDCDE310A}"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://asignaturas.fi.unam.api:8080/admin/api/nota/{id}" xr:uid="{110E4337-B225-4E20-A8B6-8917C6A4D53C}"/>
+    <hyperlink ref="B2" r:id="rId4" display="https://asignaturas.fi.unam.api:8080/api/nota/{id}" xr:uid="{8809AFD2-50AF-40C3-8061-D326B5E6A65E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEECDFE3-2A60-4EED-8F62-893D3700D171}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2946,7 +4984,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,13 +5014,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="107" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2994,9 +5032,9 @@
       <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="105"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="107"/>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
@@ -3005,27 +5043,27 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="105"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="107"/>
       <c r="D4" s="33"/>
       <c r="E4" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="105"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="107"/>
       <c r="D5" s="33"/>
       <c r="E5" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="105"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="107"/>
       <c r="D6" s="33"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -3055,15 +5093,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77F5445-FFB3-4E8A-A24C-A64D208AD4C6}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3093,13 +5131,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="111" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="32" t="s">
@@ -3110,9 +5148,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="107"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="109"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="32" t="s">
         <v>24</v>
       </c>
@@ -3121,72 +5159,72 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="107"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="109"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="33"/>
       <c r="E4" s="32" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="107"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="109"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="33"/>
       <c r="E5" s="32" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
-      <c r="B6" s="110"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="33"/>
       <c r="E6" s="32" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="37"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="112"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="34"/>
       <c r="E7" s="32" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="37"/>
+      <c r="A8" s="109"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="34"/>
       <c r="E8" s="32" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="37"/>
+      <c r="A9" s="109"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="34"/>
-      <c r="E9" s="112" t="s">
+      <c r="E9" s="37" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="37"/>
+      <c r="A10" s="109"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="34"/>
       <c r="E10" s="32" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="108"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="34"/>
       <c r="E11" s="32" t="s">
         <v>11</v>
@@ -3247,13 +5285,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3264,36 +5302,36 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -3351,13 +5389,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3368,9 +5406,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3379,31 +5417,31 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -3463,13 +5501,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="60" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3480,9 +5518,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="59"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3491,98 +5529,98 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="59"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="59"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="59"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="59"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="49" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -3593,9 +5631,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="48"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
@@ -3604,58 +5642,58 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="48"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="48"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="48"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="29" t="s">
         <v>103</v>
       </c>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="29" t="s">
         <v>104</v>
       </c>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="58" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -3666,9 +5704,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="57"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
@@ -3738,13 +5776,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3755,9 +5793,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="69"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
@@ -3766,22 +5804,22 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="70"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3792,9 +5830,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="70"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -3855,13 +5893,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3872,9 +5910,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="69"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
@@ -3883,36 +5921,36 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="69"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="69"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="69"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="70"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
@@ -3969,13 +6007,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3986,53 +6024,53 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -4043,9 +6081,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="69"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
@@ -4054,22 +6092,22 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="49" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -4080,9 +6118,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="48"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
@@ -4091,31 +6129,31 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="86"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="48"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -4126,9 +6164,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="4" t="s">
         <v>8</v>
       </c>
@@ -4172,7 +6210,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,13 +6240,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4219,9 +6257,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
@@ -4230,13 +6268,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
@@ -4245,9 +6283,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
@@ -4256,35 +6294,35 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -4295,9 +6333,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="69"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
@@ -4306,31 +6344,31 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="69"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="69"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="92" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -4341,9 +6379,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="91"/>
+      <c r="A13" s="97"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="93"/>
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
@@ -4352,40 +6390,40 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="91"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="97"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="96"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="91"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="93"/>
       <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -4396,9 +6434,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="76"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="4" t="s">
         <v>8</v>
       </c>
@@ -4475,13 +6513,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4492,9 +6530,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
@@ -4506,10 +6544,10 @@
       <c r="A4" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
@@ -4519,52 +6557,52 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="102"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="100"/>
-      <c r="C7" s="37"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="97"/>
-      <c r="C8" s="38"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="70" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -4575,9 +6613,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="69"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
@@ -4586,31 +6624,31 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="69"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="81"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="69"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="103" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="92" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -4621,9 +6659,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="91"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
@@ -4632,40 +6670,40 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="97"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="91"/>
+      <c r="A16" s="97"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="93"/>
       <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="91"/>
+      <c r="A17" s="97"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="93"/>
       <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -4676,9 +6714,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="76"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
@@ -4688,13 +6726,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C13:C17"/>
@@ -4704,6 +6735,13 @@
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{19766D17-2256-47E9-986D-0001E3F5E42D}"/>

</xml_diff>